<commit_message>
added scrolbar and logout option
</commit_message>
<xml_diff>
--- a/db/user.xlsx
+++ b/db/user.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GECKO\git-projects\Library management\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA81496D-C37A-4144-A9C7-FED55DB281A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F366CC-152F-4083-B32E-5130014221DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5670" yWindow="2445" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3000" yWindow="2520" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="59">
   <si>
     <t>ID</t>
   </si>
@@ -71,13 +71,139 @@
   </si>
   <si>
     <t>A0446457854</t>
+  </si>
+  <si>
+    <t>A000003</t>
+  </si>
+  <si>
+    <t>A0446457855</t>
+  </si>
+  <si>
+    <t>15-2-2024</t>
+  </si>
+  <si>
+    <t>A000004</t>
+  </si>
+  <si>
+    <t>A0446457856</t>
+  </si>
+  <si>
+    <t>15-2-2025</t>
+  </si>
+  <si>
+    <t>A000005</t>
+  </si>
+  <si>
+    <t>A0446457857</t>
+  </si>
+  <si>
+    <t>15-2-2026</t>
+  </si>
+  <si>
+    <t>A000006</t>
+  </si>
+  <si>
+    <t>A0446457858</t>
+  </si>
+  <si>
+    <t>15-2-2027</t>
+  </si>
+  <si>
+    <t>A000007</t>
+  </si>
+  <si>
+    <t>A0446457859</t>
+  </si>
+  <si>
+    <t>15-2-2028</t>
+  </si>
+  <si>
+    <t>A000008</t>
+  </si>
+  <si>
+    <t>A0446457860</t>
+  </si>
+  <si>
+    <t>15-2-2029</t>
+  </si>
+  <si>
+    <t>A000009</t>
+  </si>
+  <si>
+    <t>A0446457861</t>
+  </si>
+  <si>
+    <t>15-2-2030</t>
+  </si>
+  <si>
+    <t>A000010</t>
+  </si>
+  <si>
+    <t>A0446457862</t>
+  </si>
+  <si>
+    <t>15-2-2031</t>
+  </si>
+  <si>
+    <t>A000011</t>
+  </si>
+  <si>
+    <t>A0446457863</t>
+  </si>
+  <si>
+    <t>15-2-2032</t>
+  </si>
+  <si>
+    <t>A000012</t>
+  </si>
+  <si>
+    <t>A0446457864</t>
+  </si>
+  <si>
+    <t>15-2-2033</t>
+  </si>
+  <si>
+    <t>A000013</t>
+  </si>
+  <si>
+    <t>A0446457865</t>
+  </si>
+  <si>
+    <t>15-2-2034</t>
+  </si>
+  <si>
+    <t>A000014</t>
+  </si>
+  <si>
+    <t>A0446457866</t>
+  </si>
+  <si>
+    <t>15-2-2035</t>
+  </si>
+  <si>
+    <t>A000015</t>
+  </si>
+  <si>
+    <t>A0446457867</t>
+  </si>
+  <si>
+    <t>15-2-2036</t>
+  </si>
+  <si>
+    <t>A000016</t>
+  </si>
+  <si>
+    <t>A0446457868</t>
+  </si>
+  <si>
+    <t>15-2-2037</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,6 +215,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -419,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,7 +622,528 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" t="s">
+        <v>57</v>
+      </c>
+      <c r="E27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" t="s">
+        <v>57</v>
+      </c>
+      <c r="E29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
found a bug which made scrlbar invis
</commit_message>
<xml_diff>
--- a/db/user.xlsx
+++ b/db/user.xlsx
@@ -468,22 +468,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>000041</t>
+          <t>000023</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>salam</t>
+          <t>yoosef</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>valaei</t>
+          <t>faseehee</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0795435807</t>
+          <t>1296704949</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -493,29 +493,29 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2023-16-10</t>
+          <t>2023-16-3</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000023</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>salam</t>
+          <t>yusef</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>fasihi</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>1296704949</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -537,12 +537,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>dasfasdfasdf</t>
+          <t>yusef</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ilia</t>
+          <t>fasihi</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -564,54 +564,54 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000023</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>salam</t>
+          <t>yusef</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>fasihi</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>1296704949</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>09307637377</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2023-17-13</t>
+          <t>2023-16-3</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>000041</t>
+          <t>000023</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ilia</t>
+          <t>yusef</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>valaei</t>
+          <t>fasihi</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0795435807</t>
+          <t>1296704949</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -621,29 +621,29 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2023-16-10</t>
+          <t>2023-16-3</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000023</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>yusef</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>fasihi</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>1296704949</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -692,54 +692,54 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000023</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>yusef</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>fasihi</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>1296704949</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>09307637377</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2023-17-14</t>
+          <t>2023-16-3</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>000041</t>
+          <t>000023</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ilia</t>
+          <t>yusef</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>valaei</t>
+          <t>fasihi</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0795435807</t>
+          <t>1296704949</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -749,29 +749,29 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2023-16-10</t>
+          <t>2023-16-3</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000023</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>yusef</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>fasihi</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>1296704949</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -820,54 +820,54 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000023</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>yusef</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>fasihi</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>1296704949</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>09307637377</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2023-17-15</t>
+          <t>2023-16-3</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>000041</t>
+          <t>000023</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ilia</t>
+          <t>yusef</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>valaei</t>
+          <t>fasihi</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0795435807</t>
+          <t>1296704949</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -877,29 +877,29 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2023-16-10</t>
+          <t>2023-16-3</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000023</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>yusef</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>fasihi</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>1296704949</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -948,54 +948,54 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000023</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>yusef</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>fasihi</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>1296704949</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>09307637377</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2023-17-16</t>
+          <t>2023-16-3</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>000041</t>
+          <t>000023</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>ilia</t>
+          <t>yusef</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>valaei</t>
+          <t>fasihi</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0795435807</t>
+          <t>1296704949</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1005,29 +1005,29 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2023-16-10</t>
+          <t>2023-16-3</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000023</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>yusef</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>fasihi</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>1296704949</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1076,54 +1076,54 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000023</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>yusef</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>fasihi</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>1296704949</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>09307637377</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2023-17-17</t>
+          <t>2023-16-3</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>000041</t>
+          <t>000023</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>ilia</t>
+          <t>yusef</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>valaei</t>
+          <t>fasihi</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0795435807</t>
+          <t>1296704949</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1133,29 +1133,29 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2023-16-10</t>
+          <t>2023-16-3</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000023</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>yusef</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>fasihi</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>1296704949</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1204,54 +1204,54 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000023</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>yusef</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>fasihi</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>1296704949</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>09307637377</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2023-17-18</t>
+          <t>2023-16-3</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>000041</t>
+          <t>000023</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ilia</t>
+          <t>yusef</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>valaei</t>
+          <t>fasihi</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>0795435807</t>
+          <t>1296704949</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1261,29 +1261,29 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2023-16-10</t>
+          <t>2023-16-3</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000023</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>yusef</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>fasihi</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>1296704949</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1332,54 +1332,54 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000023</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>yusef</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>fasihi</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>1296704949</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>09307637377</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2023-17-19</t>
+          <t>2023-16-3</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>000041</t>
+          <t>000023</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ilia</t>
+          <t>yusef</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>valaei</t>
+          <t>fasihi</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0795435807</t>
+          <t>1296704949</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1389,29 +1389,29 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2023-16-10</t>
+          <t>2023-16-3</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000023</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>yusef</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>fasihi</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>1296704949</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1433,12 +1433,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>dasfasdfasdf</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>ilia</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1485,103 +1485,103 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2023-17-20</t>
+          <t>2023-17-37</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>000041</t>
+          <t>000057</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>ilia</t>
+          <t>bahar</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>valaei</t>
+          <t>mansoori</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0795435807</t>
+          <t>1639850817</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>09586395388</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2023-16-10</t>
+          <t>2023-17-40</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000057</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>bahar</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>mansoori</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>1639850817</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>09586395388</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>2023-17-17</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000057</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>bahar</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>mansoori</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>1639850817</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>09586395388</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>2023-17-19</t>
         </is>
       </c>
     </row>
@@ -1613,103 +1613,103 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2023-17-21</t>
+          <t>2023-17-38</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>000041</t>
+          <t>000057</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>ilia</t>
+          <t>bahar</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>valaei</t>
+          <t>mansoori</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>0795435807</t>
+          <t>1639850817</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>09586395388</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2023-16-10</t>
+          <t>2023-17-20</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000057</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>bahar</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>mansoori</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>1639850817</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>09586395388</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>2023-17-43</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000057</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>bahar</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>mansoori</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>1639850817</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>09586395388</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>2023-17-35</t>
         </is>
       </c>
     </row>
@@ -1741,103 +1741,103 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2023-17-22</t>
+          <t>2023-17-21</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>000041</t>
+          <t>000057</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>ilia</t>
+          <t>bahar</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>valaei</t>
+          <t>mansoori</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>0795435807</t>
+          <t>1639850817</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>09586395388</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2023-16-10</t>
+          <t>2023-17-31</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000057</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>bahar</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>mansoori</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>1639850817</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>09586395388</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>2023-17-16</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000057</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>bahar</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>mansoori</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>1639850817</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>09586395388</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>2023-17-22</t>
         </is>
       </c>
     </row>
@@ -1869,103 +1869,103 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2023-17-23</t>
+          <t>2023-17-36</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>000041</t>
+          <t>000057</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>ilia</t>
+          <t>bahar</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>valaei</t>
+          <t>mansoori</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>0795435807</t>
+          <t>1639850817</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>09586395388</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2023-16-10</t>
+          <t>2023-17-15</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000057</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>bahar</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>mansoori</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>1639850817</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>09586395388</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>2023-17-33</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000057</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>bahar</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>mansoori</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>1639850817</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>09586395388</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>2023-17-18</t>
         </is>
       </c>
     </row>
@@ -1997,103 +1997,103 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2023-17-24</t>
+          <t>2023-17-28</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>000041</t>
+          <t>000057</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>ilia</t>
+          <t>bahar</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>valaei</t>
+          <t>mansoori</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>0795435807</t>
+          <t>1639850817</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>09586395388</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2023-16-10</t>
+          <t>2023-17-26</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000057</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>bahar</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>mansoori</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>1639850817</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>09586395388</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>2023-17-42</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000057</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>bahar</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>mansoori</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>1639850817</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>09586395388</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>2023-17-29</t>
         </is>
       </c>
     </row>
@@ -2125,103 +2125,103 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>2023-17-25</t>
+          <t>2023-17-27</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>000041</t>
+          <t>000057</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>ilia</t>
+          <t>bahar</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>valaei</t>
+          <t>mansoori</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>0795435807</t>
+          <t>1639850817</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>09586395388</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2023-16-10</t>
+          <t>2023-17-14</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000057</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>bahar</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>mansoori</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>1639850817</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>09586395388</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>2023-17-25</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000057</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>bahar</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>mansoori</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>1639850817</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>09586395388</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>2023-17-24</t>
         </is>
       </c>
     </row>
@@ -2253,103 +2253,103 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>2023-17-26</t>
+          <t>2023-17-41</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>000041</t>
+          <t>000057</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>ilia</t>
+          <t>bahar</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>valaei</t>
+          <t>mansoori</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>0795435807</t>
+          <t>1639850817</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>09586395388</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>2023-16-10</t>
+          <t>2023-17-34</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000057</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>bahar</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>mansoori</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>1639850817</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>09586395388</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>2023-17-30</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000057</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>bahar</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>mansoori</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>1639850817</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>09586395388</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>2023-17-39</t>
         </is>
       </c>
     </row>
@@ -2361,7 +2361,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>salam</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2381,93 +2381,93 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>2023-17-27</t>
+          <t>2023-17-13</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>000041</t>
+          <t>000057</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>ilia</t>
+          <t>bahar</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>valaei</t>
+          <t>mansoori</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>0795435807</t>
+          <t>1639850817</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>09586395388</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>2023-16-10</t>
+          <t>2023-17-32</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000057</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>bahar</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>mansoori</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>1639850817</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>09586395388</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>2023-17-23</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000019</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>mamad</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>moshtagh</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>2533342179</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
@@ -2484,54 +2484,54 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000019</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>mamad</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>moshtagh</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>2533342179</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>09307637377</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>2023-17-28</t>
+          <t>2023-16-3</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>000041</t>
+          <t>000019</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>ilia</t>
+          <t>mamad</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>valaei</t>
+          <t>moshtagh</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>0795435807</t>
+          <t>2533342179</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -2541,7 +2541,7 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>2023-16-10</t>
+          <t>2023-16-3</t>
         </is>
       </c>
     </row>
@@ -2580,22 +2580,22 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000019</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>mamad</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>moshtagh</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>2533342179</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -2612,54 +2612,54 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000019</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>mamad</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>moshtagh</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>2533342179</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>09307637377</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>2023-17-29</t>
+          <t>2023-16-3</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>000041</t>
+          <t>000019</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>ilia</t>
+          <t>mamad</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>valaei</t>
+          <t>moshtagh</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>0795435807</t>
+          <t>2533342179</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -2669,7 +2669,7 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>2023-16-10</t>
+          <t>2023-16-3</t>
         </is>
       </c>
     </row>
@@ -2708,22 +2708,22 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000019</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>mamad</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>moshtagh</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>2533342179</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -2740,54 +2740,54 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000019</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>mamad</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>moshtagh</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>2533342179</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>09307637377</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>2023-17-30</t>
+          <t>2023-16-3</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>000041</t>
+          <t>000019</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>ilia</t>
+          <t>mamad</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>valaei</t>
+          <t>moshtagh</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>0795435807</t>
+          <t>2533342179</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -2797,7 +2797,7 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>2023-16-10</t>
+          <t>2023-16-3</t>
         </is>
       </c>
     </row>
@@ -2836,22 +2836,22 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000019</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>mamad</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>moshtagh</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>2533342179</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -2868,54 +2868,54 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000019</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t xml:space="preserve">mohammad </t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>moshtagh</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>2533342179</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>09307637377</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>2023-17-31</t>
+          <t>2023-16-3</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>000041</t>
+          <t>000019</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>ilia</t>
+          <t>mamad</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>valaei</t>
+          <t>moshtagh</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>0795435807</t>
+          <t>2533342179</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
@@ -2925,7 +2925,7 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>2023-16-10</t>
+          <t>2023-16-3</t>
         </is>
       </c>
     </row>
@@ -2964,22 +2964,22 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000019</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>mamad</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>moshtagh</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>2533342179</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
@@ -2996,54 +2996,54 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000019</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>mamad</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>moshtagh</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>2533342179</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>09307637377</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>2023-17-32</t>
+          <t>2023-16-3</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>000041</t>
+          <t>000019</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>ilia</t>
+          <t>mamad</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>valaei</t>
+          <t>moshtagh</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>0795435807</t>
+          <t>2533342179</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
@@ -3053,7 +3053,7 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>2023-16-10</t>
+          <t>2023-16-3</t>
         </is>
       </c>
     </row>
@@ -3092,22 +3092,22 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000019</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>mamad</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>moshtagh</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>2533342179</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
@@ -3124,54 +3124,54 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000019</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>mamad</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>moshtagh</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>2533342179</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>09307637377</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>2023-17-33</t>
+          <t>2023-16-3</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>000041</t>
+          <t>000019</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>ilia</t>
+          <t>mamad</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>valaei</t>
+          <t>moshtagh</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>0795435807</t>
+          <t>2533342179</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
@@ -3181,7 +3181,7 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>2023-16-10</t>
+          <t>2023-16-3</t>
         </is>
       </c>
     </row>
@@ -3220,22 +3220,22 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000019</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>mamad</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>moshtagh</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>2533342179</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
@@ -3252,54 +3252,54 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000019</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>mamad</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>moshtagh</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>2533342179</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>09307637377</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>2023-17-34</t>
+          <t>2023-16-3</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>000041</t>
+          <t>000019</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>ilia</t>
+          <t>mamad</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>valaei</t>
+          <t>moshtagh</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>0795435807</t>
+          <t>2533342179</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
@@ -3309,7 +3309,7 @@
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>2023-16-10</t>
+          <t>2023-16-3</t>
         </is>
       </c>
     </row>
@@ -3348,22 +3348,22 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000019</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>mamad</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>moshtagh</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>2533342179</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
@@ -3380,54 +3380,54 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000019</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>mamad</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>moshtagh</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>2533342179</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>09307637377</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>2023-17-35</t>
+          <t>2023-16-3</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>000041</t>
+          <t>000019</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>ilia</t>
+          <t>mamad</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>valaei</t>
+          <t>moshtagh</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>0795435807</t>
+          <t>2533342179</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
@@ -3437,29 +3437,29 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>2023-16-10</t>
+          <t>2023-16-3</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000041</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>ilia</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>valaei</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>0795435807</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
@@ -3469,29 +3469,29 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>2023-16-10</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000041</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>ilia</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>valaei</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>0795435807</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
@@ -3501,39 +3501,39 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>2023-16-10</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000041</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>ilia</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>valaei</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>0795435807</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>09307637377</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>2023-17-36</t>
+          <t>2023-16-10</t>
         </is>
       </c>
     </row>
@@ -3572,22 +3572,22 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000041</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>ilia</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>valaei</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>0795435807</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
@@ -3597,29 +3597,29 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>2023-16-10</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000041</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>ilia</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>valaei</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>0795435807</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
@@ -3629,39 +3629,39 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>2023-16-10</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000041</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>ilia</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>valaei</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>0795435807</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>09307637377</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>2023-17-37</t>
+          <t>2023-16-10</t>
         </is>
       </c>
     </row>
@@ -3700,22 +3700,22 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000041</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>ilia</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>valaei</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>0795435807</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
@@ -3725,29 +3725,29 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>2023-16-10</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000041</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>ilia</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>valaei</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>0795435807</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
@@ -3757,39 +3757,39 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>2023-16-10</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000041</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>ilia</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>valaei</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>0795435807</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>09307637377</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>2023-17-38</t>
+          <t>2023-16-10</t>
         </is>
       </c>
     </row>
@@ -3828,22 +3828,22 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000041</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>ilia</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>valaei</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>0795435807</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
@@ -3853,29 +3853,29 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>2023-16-10</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000041</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>ilia</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>valaei</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>0795435807</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
@@ -3885,39 +3885,39 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>2023-16-10</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000041</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>ilia</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>valaei</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>0795435807</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>09307637377</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>2023-17-39</t>
+          <t>2023-16-10</t>
         </is>
       </c>
     </row>
@@ -3956,22 +3956,22 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000041</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>ilia</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>valaei</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>0795435807</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
@@ -3981,29 +3981,29 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>2023-16-10</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000041</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>ilia</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>valaei</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>0795435807</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
@@ -4013,39 +4013,39 @@
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>2023-16-10</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000041</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>ilia</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>valaei</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>0795435807</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>09307637377</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>2023-17-40</t>
+          <t>2023-16-10</t>
         </is>
       </c>
     </row>
@@ -4084,22 +4084,22 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000041</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>ilia</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>valaei</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>0795435807</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
@@ -4109,29 +4109,29 @@
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>2023-16-10</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000041</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>ilia</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>valaei</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>0795435807</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
@@ -4141,39 +4141,39 @@
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>2023-16-10</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000041</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>ilia</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>valaei</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>0795435807</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>09307637377</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>2023-17-41</t>
+          <t>2023-16-10</t>
         </is>
       </c>
     </row>
@@ -4212,22 +4212,22 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000041</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>ilia</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>valaei</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>0795435807</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
@@ -4237,29 +4237,29 @@
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>2023-16-10</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000041</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>ilia</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>valaei</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>0795435807</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
@@ -4269,39 +4269,39 @@
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>2023-16-10</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000041</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>ilia</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>valaei</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>0795435807</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>09307637377</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>2023-17-42</t>
+          <t>2023-16-10</t>
         </is>
       </c>
     </row>
@@ -4340,22 +4340,22 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000041</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>ilia</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>valaei</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>0795435807</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
@@ -4365,29 +4365,29 @@
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>2023-16-10</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000041</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>ilia</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>valaei</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>0795435807</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
@@ -4397,39 +4397,39 @@
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>2023-16-10</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000041</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>salam</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>valaei</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>0795435807</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>09307637377</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>2023-17-43</t>
+          <t>2023-16-10</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added a delete function but need to work on
</commit_message>
<xml_diff>
--- a/db/user.xlsx
+++ b/db/user.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F125"/>
+  <dimension ref="A1:F84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,1312 +468,1312 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000003</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>yoosef</t>
+          <t>Margaret</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>faseehee</t>
+          <t>Christine</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000004</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>Judith</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>Julie</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000010</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>Barbara</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>Wendy</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000013</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>Anne</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>Linda</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000014</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>Karen</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>Robyn</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000015</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>Judith</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000016</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>Diane</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>Mary</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000017</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>Sandra</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000018</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>Wendy</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>Margaret</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000019</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>Janet</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>Patricia</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000020</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>Heather</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>Debra</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000024</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>Julie</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>Anne</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000025</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>Suzanne</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>Catherine</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000026</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>Lorraine</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>Diane</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000029</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>Rosemary</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>Suzanne</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000030</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>Raewyn</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>Vicki</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000031</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>Kathleen</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>Michelle</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000032</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>Pauline</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>Carolyn</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000034</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>Gail</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>Fiona</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000035</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>Denise</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>Raewyn</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000036</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>Sharon</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>Kathryn</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000037</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>Lesley</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>Alison</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000038</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>Yvonne</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>Janet</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000039</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>Catherine</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>Pamela</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000040</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>Shirley</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>Jacqueline</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000041</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>Beverley</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>Dianne</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000042</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>Maureen</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>Yvonne</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000043</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>Deborah</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>Rosemary</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000044</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>Jillian</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>Kathleen</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000045</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>yusef</t>
+          <t>Ann</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>fasihi</t>
+          <t>Janice</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>000023</t>
+          <t>000046</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>dasfasdfasdf</t>
+          <t>Annette</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>ilia</t>
+          <t>Brenda</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1296704949</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000047</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>Colleen</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>Shirley</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2023-17-37</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000048</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>Jane</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>Nicola</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2023-17-40</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000049</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>Marie</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>Pauline</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2023-17-17</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000050</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>Sheryl</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>Annette</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2023-17-19</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000051</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>Carolyn</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>Angela</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2023-17-38</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000052</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>Frances</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2023-17-20</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000053</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>Kathryn</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>Kerry</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2023-17-43</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000054</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>Kay</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>Lorraine</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2023-17-35</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000055</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>Jacqueline</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>Marie</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2023-17-21</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000056</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>Cheryl</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>Jillian</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2023-17-31</t>
+          <t>s</t>
         </is>
       </c>
     </row>
@@ -1785,2651 +1785,1339 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>Ruth</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>Jan</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2023-17-16</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000058</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>Glenda</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>Sheryl</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2023-17-22</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000059</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>Maria</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>Cheryl</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2023-17-36</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000060</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>Sally</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>Andrea</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2023-17-15</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000061</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>Lynda</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>Ann</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2023-17-33</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000062</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>Lynne</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>Lynda</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2023-17-18</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000063</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>Marion</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>Maree</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2023-17-28</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000064</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>Gillian</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>Maria</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2023-17-26</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000065</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>Glenys</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>Gillian</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2023-17-42</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000066</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>Jan</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>Kay</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2023-17-29</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000067</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>Jeanette</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>Lesley</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>2023-17-27</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000068</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>Elaine</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>Sally</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2023-17-14</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000069</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>Irene</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>Shona</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2023-17-25</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000070</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>Jocelyn</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>Stephanie</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>2023-17-24</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000071</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>Donna</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>Frances</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>2023-17-41</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000072</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>Brenda</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>Louise</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>2023-17-34</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000073</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>Vicki</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>Caroline</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>2023-17-30</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000074</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>Josephine</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>Vivienne</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>2023-17-39</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000075</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>salam</t>
+          <t>Jill</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>Colleen</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>2023-17-13</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000076</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>Angela</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>Gail</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>2023-17-32</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000077</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>bahar</t>
+          <t>Vivienne</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>mansoori</t>
+          <t>Michele</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>1639850817</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>09586395388</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>2023-17-23</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000078</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>Valerie</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>Diana</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000079</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>Shona</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>Ruth</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000080</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>Joanne</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>Bronwyn</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000081</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>Joy</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>Beverley</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000082</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>Lois</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>Debbie</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000083</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>Stephanie</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>Lynne</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000084</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>Joan</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>Sarah</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000085</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>Dorothy</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>Shelley</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000086</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>Paula</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>Glenda</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000087</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>Diana</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>Jeanette</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000088</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>Gloria</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>Janine</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000089</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>Adrienne</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>Teresa</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000090</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>Bronwyn</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>Anna</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000091</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t xml:space="preserve">mohammad </t>
+          <t>Marian</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>Maureen</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000092</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>Lynnette</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>s</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000093</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>Louise</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>s</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000094</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>Virginia</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>s</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000095</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>Penelope</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>s</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000096</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>Lynn</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>s</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000097</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>Christina</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>s</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
+          <t>s</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>s</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>mamad</t>
+          <t>Claire</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>moshtagh</t>
+          <t>s</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>2533342179</t>
+          <t>s</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>09307637377</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>2023-16-3</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>000019</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>mamad</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>moshtagh</t>
-        </is>
-      </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>2533342179</t>
-        </is>
-      </c>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F85" t="inlineStr">
-        <is>
-          <t>2023-16-3</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>000019</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>mamad</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>moshtagh</t>
-        </is>
-      </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>2533342179</t>
-        </is>
-      </c>
-      <c r="E86" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F86" t="inlineStr">
-        <is>
-          <t>2023-16-3</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>000019</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>mamad</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>moshtagh</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>2533342179</t>
-        </is>
-      </c>
-      <c r="E87" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F87" t="inlineStr">
-        <is>
-          <t>2023-16-3</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>000019</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>mamad</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>moshtagh</t>
-        </is>
-      </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>2533342179</t>
-        </is>
-      </c>
-      <c r="E88" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F88" t="inlineStr">
-        <is>
-          <t>2023-16-3</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>000019</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>mamad</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>moshtagh</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>2533342179</t>
-        </is>
-      </c>
-      <c r="E89" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F89" t="inlineStr">
-        <is>
-          <t>2023-16-3</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>000019</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>mamad</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>moshtagh</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>2533342179</t>
-        </is>
-      </c>
-      <c r="E90" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>2023-16-3</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>000019</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>mamad</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>moshtagh</t>
-        </is>
-      </c>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>2533342179</t>
-        </is>
-      </c>
-      <c r="E91" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F91" t="inlineStr">
-        <is>
-          <t>2023-16-3</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>000019</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>mamad</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>moshtagh</t>
-        </is>
-      </c>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>2533342179</t>
-        </is>
-      </c>
-      <c r="E92" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F92" t="inlineStr">
-        <is>
-          <t>2023-16-3</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>000019</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>mamad</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>moshtagh</t>
-        </is>
-      </c>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t>2533342179</t>
-        </is>
-      </c>
-      <c r="E93" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F93" t="inlineStr">
-        <is>
-          <t>2023-16-3</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>000019</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>mamad</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>moshtagh</t>
-        </is>
-      </c>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t>2533342179</t>
-        </is>
-      </c>
-      <c r="E94" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F94" t="inlineStr">
-        <is>
-          <t>2023-16-3</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>000041</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>ilia</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>valaei</t>
-        </is>
-      </c>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>0795435807</t>
-        </is>
-      </c>
-      <c r="E95" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F95" t="inlineStr">
-        <is>
-          <t>2023-16-10</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>000041</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>ilia</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>valaei</t>
-        </is>
-      </c>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>0795435807</t>
-        </is>
-      </c>
-      <c r="E96" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F96" t="inlineStr">
-        <is>
-          <t>2023-16-10</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>000041</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>ilia</t>
-        </is>
-      </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>valaei</t>
-        </is>
-      </c>
-      <c r="D97" t="inlineStr">
-        <is>
-          <t>0795435807</t>
-        </is>
-      </c>
-      <c r="E97" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F97" t="inlineStr">
-        <is>
-          <t>2023-16-10</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>000041</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>ilia</t>
-        </is>
-      </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>valaei</t>
-        </is>
-      </c>
-      <c r="D98" t="inlineStr">
-        <is>
-          <t>0795435807</t>
-        </is>
-      </c>
-      <c r="E98" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F98" t="inlineStr">
-        <is>
-          <t>2023-16-10</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>000041</t>
-        </is>
-      </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>ilia</t>
-        </is>
-      </c>
-      <c r="C99" t="inlineStr">
-        <is>
-          <t>valaei</t>
-        </is>
-      </c>
-      <c r="D99" t="inlineStr">
-        <is>
-          <t>0795435807</t>
-        </is>
-      </c>
-      <c r="E99" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F99" t="inlineStr">
-        <is>
-          <t>2023-16-10</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>000041</t>
-        </is>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>ilia</t>
-        </is>
-      </c>
-      <c r="C100" t="inlineStr">
-        <is>
-          <t>valaei</t>
-        </is>
-      </c>
-      <c r="D100" t="inlineStr">
-        <is>
-          <t>0795435807</t>
-        </is>
-      </c>
-      <c r="E100" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F100" t="inlineStr">
-        <is>
-          <t>2023-16-10</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>000041</t>
-        </is>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>ilia</t>
-        </is>
-      </c>
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>valaei</t>
-        </is>
-      </c>
-      <c r="D101" t="inlineStr">
-        <is>
-          <t>0795435807</t>
-        </is>
-      </c>
-      <c r="E101" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F101" t="inlineStr">
-        <is>
-          <t>2023-16-10</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>000041</t>
-        </is>
-      </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>ilia</t>
-        </is>
-      </c>
-      <c r="C102" t="inlineStr">
-        <is>
-          <t>valaei</t>
-        </is>
-      </c>
-      <c r="D102" t="inlineStr">
-        <is>
-          <t>0795435807</t>
-        </is>
-      </c>
-      <c r="E102" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F102" t="inlineStr">
-        <is>
-          <t>2023-16-10</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="inlineStr">
-        <is>
-          <t>000041</t>
-        </is>
-      </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>ilia</t>
-        </is>
-      </c>
-      <c r="C103" t="inlineStr">
-        <is>
-          <t>valaei</t>
-        </is>
-      </c>
-      <c r="D103" t="inlineStr">
-        <is>
-          <t>0795435807</t>
-        </is>
-      </c>
-      <c r="E103" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F103" t="inlineStr">
-        <is>
-          <t>2023-16-10</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>000041</t>
-        </is>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>ilia</t>
-        </is>
-      </c>
-      <c r="C104" t="inlineStr">
-        <is>
-          <t>valaei</t>
-        </is>
-      </c>
-      <c r="D104" t="inlineStr">
-        <is>
-          <t>0795435807</t>
-        </is>
-      </c>
-      <c r="E104" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F104" t="inlineStr">
-        <is>
-          <t>2023-16-10</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="inlineStr">
-        <is>
-          <t>000041</t>
-        </is>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>ilia</t>
-        </is>
-      </c>
-      <c r="C105" t="inlineStr">
-        <is>
-          <t>valaei</t>
-        </is>
-      </c>
-      <c r="D105" t="inlineStr">
-        <is>
-          <t>0795435807</t>
-        </is>
-      </c>
-      <c r="E105" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F105" t="inlineStr">
-        <is>
-          <t>2023-16-10</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="inlineStr">
-        <is>
-          <t>000041</t>
-        </is>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>ilia</t>
-        </is>
-      </c>
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>valaei</t>
-        </is>
-      </c>
-      <c r="D106" t="inlineStr">
-        <is>
-          <t>0795435807</t>
-        </is>
-      </c>
-      <c r="E106" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F106" t="inlineStr">
-        <is>
-          <t>2023-16-10</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>000041</t>
-        </is>
-      </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>ilia</t>
-        </is>
-      </c>
-      <c r="C107" t="inlineStr">
-        <is>
-          <t>valaei</t>
-        </is>
-      </c>
-      <c r="D107" t="inlineStr">
-        <is>
-          <t>0795435807</t>
-        </is>
-      </c>
-      <c r="E107" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F107" t="inlineStr">
-        <is>
-          <t>2023-16-10</t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>000041</t>
-        </is>
-      </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>ilia</t>
-        </is>
-      </c>
-      <c r="C108" t="inlineStr">
-        <is>
-          <t>valaei</t>
-        </is>
-      </c>
-      <c r="D108" t="inlineStr">
-        <is>
-          <t>0795435807</t>
-        </is>
-      </c>
-      <c r="E108" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F108" t="inlineStr">
-        <is>
-          <t>2023-16-10</t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="inlineStr">
-        <is>
-          <t>000041</t>
-        </is>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>ilia</t>
-        </is>
-      </c>
-      <c r="C109" t="inlineStr">
-        <is>
-          <t>valaei</t>
-        </is>
-      </c>
-      <c r="D109" t="inlineStr">
-        <is>
-          <t>0795435807</t>
-        </is>
-      </c>
-      <c r="E109" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F109" t="inlineStr">
-        <is>
-          <t>2023-16-10</t>
-        </is>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="inlineStr">
-        <is>
-          <t>000041</t>
-        </is>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>ilia</t>
-        </is>
-      </c>
-      <c r="C110" t="inlineStr">
-        <is>
-          <t>valaei</t>
-        </is>
-      </c>
-      <c r="D110" t="inlineStr">
-        <is>
-          <t>0795435807</t>
-        </is>
-      </c>
-      <c r="E110" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F110" t="inlineStr">
-        <is>
-          <t>2023-16-10</t>
-        </is>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="inlineStr">
-        <is>
-          <t>000041</t>
-        </is>
-      </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>ilia</t>
-        </is>
-      </c>
-      <c r="C111" t="inlineStr">
-        <is>
-          <t>valaei</t>
-        </is>
-      </c>
-      <c r="D111" t="inlineStr">
-        <is>
-          <t>0795435807</t>
-        </is>
-      </c>
-      <c r="E111" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F111" t="inlineStr">
-        <is>
-          <t>2023-16-10</t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="inlineStr">
-        <is>
-          <t>000041</t>
-        </is>
-      </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>ilia</t>
-        </is>
-      </c>
-      <c r="C112" t="inlineStr">
-        <is>
-          <t>valaei</t>
-        </is>
-      </c>
-      <c r="D112" t="inlineStr">
-        <is>
-          <t>0795435807</t>
-        </is>
-      </c>
-      <c r="E112" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F112" t="inlineStr">
-        <is>
-          <t>2023-16-10</t>
-        </is>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="inlineStr">
-        <is>
-          <t>000041</t>
-        </is>
-      </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>ilia</t>
-        </is>
-      </c>
-      <c r="C113" t="inlineStr">
-        <is>
-          <t>valaei</t>
-        </is>
-      </c>
-      <c r="D113" t="inlineStr">
-        <is>
-          <t>0795435807</t>
-        </is>
-      </c>
-      <c r="E113" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F113" t="inlineStr">
-        <is>
-          <t>2023-16-10</t>
-        </is>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="inlineStr">
-        <is>
-          <t>000041</t>
-        </is>
-      </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>ilia</t>
-        </is>
-      </c>
-      <c r="C114" t="inlineStr">
-        <is>
-          <t>valaei</t>
-        </is>
-      </c>
-      <c r="D114" t="inlineStr">
-        <is>
-          <t>0795435807</t>
-        </is>
-      </c>
-      <c r="E114" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F114" t="inlineStr">
-        <is>
-          <t>2023-16-10</t>
-        </is>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="inlineStr">
-        <is>
-          <t>000041</t>
-        </is>
-      </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>ilia</t>
-        </is>
-      </c>
-      <c r="C115" t="inlineStr">
-        <is>
-          <t>valaei</t>
-        </is>
-      </c>
-      <c r="D115" t="inlineStr">
-        <is>
-          <t>0795435807</t>
-        </is>
-      </c>
-      <c r="E115" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F115" t="inlineStr">
-        <is>
-          <t>2023-16-10</t>
-        </is>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="inlineStr">
-        <is>
-          <t>000041</t>
-        </is>
-      </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>ilia</t>
-        </is>
-      </c>
-      <c r="C116" t="inlineStr">
-        <is>
-          <t>valaei</t>
-        </is>
-      </c>
-      <c r="D116" t="inlineStr">
-        <is>
-          <t>0795435807</t>
-        </is>
-      </c>
-      <c r="E116" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F116" t="inlineStr">
-        <is>
-          <t>2023-16-10</t>
-        </is>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" t="inlineStr">
-        <is>
-          <t>000041</t>
-        </is>
-      </c>
-      <c r="B117" t="inlineStr">
-        <is>
-          <t>ilia</t>
-        </is>
-      </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>valaei</t>
-        </is>
-      </c>
-      <c r="D117" t="inlineStr">
-        <is>
-          <t>0795435807</t>
-        </is>
-      </c>
-      <c r="E117" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F117" t="inlineStr">
-        <is>
-          <t>2023-16-10</t>
-        </is>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="inlineStr">
-        <is>
-          <t>000041</t>
-        </is>
-      </c>
-      <c r="B118" t="inlineStr">
-        <is>
-          <t>ilia</t>
-        </is>
-      </c>
-      <c r="C118" t="inlineStr">
-        <is>
-          <t>valaei</t>
-        </is>
-      </c>
-      <c r="D118" t="inlineStr">
-        <is>
-          <t>0795435807</t>
-        </is>
-      </c>
-      <c r="E118" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F118" t="inlineStr">
-        <is>
-          <t>2023-16-10</t>
-        </is>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="inlineStr">
-        <is>
-          <t>000041</t>
-        </is>
-      </c>
-      <c r="B119" t="inlineStr">
-        <is>
-          <t>ilia</t>
-        </is>
-      </c>
-      <c r="C119" t="inlineStr">
-        <is>
-          <t>valaei</t>
-        </is>
-      </c>
-      <c r="D119" t="inlineStr">
-        <is>
-          <t>0795435807</t>
-        </is>
-      </c>
-      <c r="E119" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F119" t="inlineStr">
-        <is>
-          <t>2023-16-10</t>
-        </is>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" t="inlineStr">
-        <is>
-          <t>000041</t>
-        </is>
-      </c>
-      <c r="B120" t="inlineStr">
-        <is>
-          <t>ilia</t>
-        </is>
-      </c>
-      <c r="C120" t="inlineStr">
-        <is>
-          <t>valaei</t>
-        </is>
-      </c>
-      <c r="D120" t="inlineStr">
-        <is>
-          <t>0795435807</t>
-        </is>
-      </c>
-      <c r="E120" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F120" t="inlineStr">
-        <is>
-          <t>2023-16-10</t>
-        </is>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" t="inlineStr">
-        <is>
-          <t>000041</t>
-        </is>
-      </c>
-      <c r="B121" t="inlineStr">
-        <is>
-          <t>ilia</t>
-        </is>
-      </c>
-      <c r="C121" t="inlineStr">
-        <is>
-          <t>valaei</t>
-        </is>
-      </c>
-      <c r="D121" t="inlineStr">
-        <is>
-          <t>0795435807</t>
-        </is>
-      </c>
-      <c r="E121" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F121" t="inlineStr">
-        <is>
-          <t>2023-16-10</t>
-        </is>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="inlineStr">
-        <is>
-          <t>000041</t>
-        </is>
-      </c>
-      <c r="B122" t="inlineStr">
-        <is>
-          <t>ilia</t>
-        </is>
-      </c>
-      <c r="C122" t="inlineStr">
-        <is>
-          <t>valaei</t>
-        </is>
-      </c>
-      <c r="D122" t="inlineStr">
-        <is>
-          <t>0795435807</t>
-        </is>
-      </c>
-      <c r="E122" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F122" t="inlineStr">
-        <is>
-          <t>2023-16-10</t>
-        </is>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" t="inlineStr">
-        <is>
-          <t>000041</t>
-        </is>
-      </c>
-      <c r="B123" t="inlineStr">
-        <is>
-          <t>ilia</t>
-        </is>
-      </c>
-      <c r="C123" t="inlineStr">
-        <is>
-          <t>valaei</t>
-        </is>
-      </c>
-      <c r="D123" t="inlineStr">
-        <is>
-          <t>0795435807</t>
-        </is>
-      </c>
-      <c r="E123" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F123" t="inlineStr">
-        <is>
-          <t>2023-16-10</t>
-        </is>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" t="inlineStr">
-        <is>
-          <t>000041</t>
-        </is>
-      </c>
-      <c r="B124" t="inlineStr">
-        <is>
-          <t>ilia</t>
-        </is>
-      </c>
-      <c r="C124" t="inlineStr">
-        <is>
-          <t>valaei</t>
-        </is>
-      </c>
-      <c r="D124" t="inlineStr">
-        <is>
-          <t>0795435807</t>
-        </is>
-      </c>
-      <c r="E124" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F124" t="inlineStr">
-        <is>
-          <t>2023-16-10</t>
-        </is>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" t="inlineStr">
-        <is>
-          <t>000041</t>
-        </is>
-      </c>
-      <c r="B125" t="inlineStr">
-        <is>
-          <t>salam</t>
-        </is>
-      </c>
-      <c r="C125" t="inlineStr">
-        <is>
-          <t>valaei</t>
-        </is>
-      </c>
-      <c r="D125" t="inlineStr">
-        <is>
-          <t>0795435807</t>
-        </is>
-      </c>
-      <c r="E125" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F125" t="inlineStr">
-        <is>
-          <t>2023-16-10</t>
+          <t>s</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
tried to fix remove function but doesnt seems to work
</commit_message>
<xml_diff>
--- a/db/user.xlsx
+++ b/db/user.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F84"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,17 +468,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>000003</t>
+          <t>000081</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Margaret</t>
+          <t>Joy</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Christine</t>
+          <t>Beverley</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -500,17 +500,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>000004</t>
+          <t>000046</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Judith</t>
+          <t>Annette</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Julie</t>
+          <t>Brenda</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -532,17 +532,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>000010</t>
+          <t>000080</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Barbara</t>
+          <t>Joanne</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Wendy</t>
+          <t>Bronwyn</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -564,17 +564,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>000013</t>
+          <t>000073</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Anne</t>
+          <t>Vicki</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Linda</t>
+          <t>Caroline</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -596,17 +596,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>000014</t>
+          <t>000032</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Karen</t>
+          <t>Pauline</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Robyn</t>
+          <t>Carolyn</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -628,17 +628,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>000015</t>
+          <t>000025</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Suzanne</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Judith</t>
+          <t>Catherine</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -660,17 +660,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>000016</t>
+          <t>000059</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Diane</t>
+          <t>Maria</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Mary</t>
+          <t>Cheryl</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -692,17 +692,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>000017</t>
+          <t>000075</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Sandra</t>
+          <t>Jill</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Colleen</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -724,17 +724,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>000018</t>
+          <t>000020</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Wendy</t>
+          <t>Heather</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Margaret</t>
+          <t>Debra</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -756,17 +756,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000078</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Janet</t>
+          <t>Valerie</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>Diana</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -788,17 +788,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>000020</t>
+          <t>000026</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Heather</t>
+          <t>Lorraine</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Debra</t>
+          <t>Diane</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -820,17 +820,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>000024</t>
+          <t>000041</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Julie</t>
+          <t>Beverley</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Anne</t>
+          <t>Dianne</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -852,17 +852,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>000025</t>
+          <t>000034</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Suzanne</t>
+          <t>Gail</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Catherine</t>
+          <t>Fiona</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -884,17 +884,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>000026</t>
+          <t>000071</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Lorraine</t>
+          <t>Donna</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Diane</t>
+          <t>Frances</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -916,17 +916,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>000029</t>
+          <t>000076</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Rosemary</t>
+          <t>Angela</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Suzanne</t>
+          <t>Gail</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -948,17 +948,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>000030</t>
+          <t>000065</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Raewyn</t>
+          <t>Glenys</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Vicki</t>
+          <t>Gillian</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -980,17 +980,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>000031</t>
+          <t>000086</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Kathleen</t>
+          <t>Paula</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Michelle</t>
+          <t>Glenda</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1012,17 +1012,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>000032</t>
+          <t>000017</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Pauline</t>
+          <t>Sandra</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Carolyn</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1044,17 +1044,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>000034</t>
+          <t>000040</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Gail</t>
+          <t>Shirley</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Fiona</t>
+          <t>Jacqueline</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1076,17 +1076,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>000035</t>
+          <t>000057</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Denise</t>
+          <t>Ruth</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Raewyn</t>
+          <t>Jan</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1108,17 +1108,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>000036</t>
+          <t>000038</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Sharon</t>
+          <t>Yvonne</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Kathryn</t>
+          <t>Janet</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1140,17 +1140,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>000037</t>
+          <t>000045</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Lesley</t>
+          <t>Ann</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Alison</t>
+          <t>Janice</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1172,17 +1172,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>000038</t>
+          <t>000088</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Yvonne</t>
+          <t>Gloria</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Janet</t>
+          <t>Janine</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1204,17 +1204,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>000039</t>
+          <t>000087</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Catherine</t>
+          <t>Diana</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Pamela</t>
+          <t>Jeanette</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1236,17 +1236,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>000040</t>
+          <t>000056</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Shirley</t>
+          <t>Cheryl</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Jacqueline</t>
+          <t>Jillian</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1268,17 +1268,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>000041</t>
+          <t>000044</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Beverley</t>
+          <t>Jillian</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Dianne</t>
+          <t>Kathleen</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1300,17 +1300,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>000042</t>
+          <t>000036</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Maureen</t>
+          <t>Sharon</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Yvonne</t>
+          <t>Kathryn</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1332,17 +1332,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>000043</t>
+          <t>000066</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Deborah</t>
+          <t>Jan</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Rosemary</t>
+          <t>Kay</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1364,17 +1364,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>000044</t>
+          <t>000053</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Jillian</t>
+          <t>Kathryn</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Kathleen</t>
+          <t>Kerry</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1396,17 +1396,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>000045</t>
+          <t>000052</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Ann</t>
+          <t>Frances</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Janice</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1428,17 +1428,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>000046</t>
+          <t>000067</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Annette</t>
+          <t>Jeanette</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Brenda</t>
+          <t>Lesley</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1460,17 +1460,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>000047</t>
+          <t>000054</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Colleen</t>
+          <t>Kay</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Shirley</t>
+          <t>Lorraine</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1492,17 +1492,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>000048</t>
+          <t>000072</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Jane</t>
+          <t>Brenda</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Nicola</t>
+          <t>Louise</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1524,17 +1524,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>000049</t>
+          <t>000062</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Marie</t>
+          <t>Lynne</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Pauline</t>
+          <t>Lynda</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1556,17 +1556,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>000050</t>
+          <t>000083</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Sheryl</t>
+          <t>Stephanie</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Annette</t>
+          <t>Lynne</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1588,17 +1588,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>000051</t>
+          <t>000063</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Carolyn</t>
+          <t>Marion</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Angela</t>
+          <t>Maree</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1620,17 +1620,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>000052</t>
+          <t>000018</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Frances</t>
+          <t>Wendy</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Margaret</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1652,17 +1652,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>000053</t>
+          <t>000064</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Kathryn</t>
+          <t>Gillian</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Kerry</t>
+          <t>Maria</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1684,17 +1684,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>000054</t>
+          <t>000055</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Kay</t>
+          <t>Jacqueline</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Lorraine</t>
+          <t>Marie</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1716,17 +1716,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>000055</t>
+          <t>000091</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Jacqueline</t>
+          <t>Marian</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Marie</t>
+          <t>Maureen</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1748,17 +1748,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>000056</t>
+          <t>000077</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Cheryl</t>
+          <t>Vivienne</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Jillian</t>
+          <t>Michele</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1780,17 +1780,17 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>000057</t>
+          <t>000031</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Ruth</t>
+          <t>Kathleen</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Jan</t>
+          <t>Michelle</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1812,17 +1812,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>000058</t>
+          <t>000048</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Glenda</t>
+          <t>Jane</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Sheryl</t>
+          <t>Nicola</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1844,17 +1844,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>000059</t>
+          <t>000039</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Maria</t>
+          <t>Catherine</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Cheryl</t>
+          <t>Pamela</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1876,17 +1876,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>000060</t>
+          <t>000049</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Sally</t>
+          <t>Marie</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Andrea</t>
+          <t>Pauline</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1908,17 +1908,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>000061</t>
+          <t>000035</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Lynda</t>
+          <t>Denise</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Ann</t>
+          <t>Raewyn</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1940,17 +1940,17 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>000062</t>
+          <t>000014</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Lynne</t>
+          <t>Karen</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Lynda</t>
+          <t>Robyn</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1972,17 +1972,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>000063</t>
+          <t>000043</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Marion</t>
+          <t>Deborah</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Maree</t>
+          <t>Rosemary</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -2004,17 +2004,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>000064</t>
+          <t>000079</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Gillian</t>
+          <t>Shona</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Maria</t>
+          <t>Ruth</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -2036,17 +2036,17 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>000065</t>
+          <t>000068</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Glenys</t>
+          <t>Elaine</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Gillian</t>
+          <t>Sally</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -2068,17 +2068,17 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>000066</t>
+          <t>000084</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Jan</t>
+          <t>Joan</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Kay</t>
+          <t>Sarah</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -2100,17 +2100,17 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>000067</t>
+          <t>000085</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Jeanette</t>
+          <t>Dorothy</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Lesley</t>
+          <t>Shelley</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -2132,17 +2132,17 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>000068</t>
+          <t>000058</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Elaine</t>
+          <t>Glenda</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Sally</t>
+          <t>Sheryl</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -2164,17 +2164,17 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>000069</t>
+          <t>000047</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Irene</t>
+          <t>Colleen</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Shona</t>
+          <t>Shirley</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -2196,17 +2196,17 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>000070</t>
+          <t>000069</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Jocelyn</t>
+          <t>Irene</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Stephanie</t>
+          <t>Shona</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -2228,17 +2228,17 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>000071</t>
+          <t>000070</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Donna</t>
+          <t>Jocelyn</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Frances</t>
+          <t>Stephanie</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -2260,17 +2260,17 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>000072</t>
+          <t>000029</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Brenda</t>
+          <t>Rosemary</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Louise</t>
+          <t>Suzanne</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -2292,17 +2292,17 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>000073</t>
+          <t>000089</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Vicki</t>
+          <t>Adrienne</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Caroline</t>
+          <t>Teresa</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -2324,17 +2324,17 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>000074</t>
+          <t>000030</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Josephine</t>
+          <t>Raewyn</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Vivienne</t>
+          <t>Vicki</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -2356,17 +2356,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>000075</t>
+          <t>000074</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Jill</t>
+          <t>Josephine</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Colleen</t>
+          <t>Vivienne</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2388,17 +2388,17 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>000076</t>
+          <t>000042</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Angela</t>
+          <t>Maureen</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Gail</t>
+          <t>Yvonne</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -2420,17 +2420,17 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>000077</t>
+          <t>s</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Vivienne</t>
+          <t>clare</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Michele</t>
+          <t>khikhu</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2452,17 +2452,17 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>000078</t>
+          <t>000092</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Valerie</t>
+          <t>Lynnette</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Diana</t>
+          <t>s</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -2484,17 +2484,17 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>000079</t>
+          <t>000093</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Shona</t>
+          <t>Louise</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Ruth</t>
+          <t>s</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2516,17 +2516,17 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>000080</t>
+          <t>000094</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Joanne</t>
+          <t>Virginia</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Bronwyn</t>
+          <t>s</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2548,17 +2548,17 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>000081</t>
+          <t>000095</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Joy</t>
+          <t>Penelope</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Beverley</t>
+          <t>s</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2580,17 +2580,17 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>000082</t>
+          <t>000096</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Lois</t>
+          <t>Lynn</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Debbie</t>
+          <t>s</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2612,17 +2612,17 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>000083</t>
+          <t>000097</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Stephanie</t>
+          <t>Christina</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Lynne</t>
+          <t>s</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2636,486 +2636,6 @@
         </is>
       </c>
       <c r="F69" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>000084</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>Joan</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>Sarah</t>
-        </is>
-      </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>000085</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>Dorothy</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>Shelley</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="F71" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>000086</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>Paula</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>Glenda</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="F72" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>000087</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>Diana</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>Jeanette</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>000088</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>Gloria</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>Janine</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="F74" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>000089</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>Adrienne</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>Teresa</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="F75" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>000090</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>Bronwyn</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>Anna</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="E76" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="F76" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>000091</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>Marian</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>Maureen</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="F77" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>000092</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>Lynnette</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="F78" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>000093</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>Louise</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>000094</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>Virginia</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="F80" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>000095</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>Penelope</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="F81" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>000096</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>Lynn</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="F82" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>000097</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>Christina</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="F83" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>Claire</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="E84" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="F84" t="inlineStr">
         <is>
           <t>s</t>
         </is>

</xml_diff>

<commit_message>
users page is almost over(fixed all bugs)
</commit_message>
<xml_diff>
--- a/db/user.xlsx
+++ b/db/user.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,137 +434,98 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Mem ID</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0.2</t>
+          <t>NAME</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0.1</t>
+          <t>LAST NAME</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Mem ID</t>
+          <t>NUMBER</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>NAME</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>LAST NAME</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>NUMBER</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>DATE</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>507365</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>ilia</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>valaei</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0441201425</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>709156</t>
+          <t>09307637377</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>ilia</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>valaee</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>0441201425</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>02/18/2023</t>
+          <t>02/20/2023</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>557690</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>sdfgsgsdf</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>gsdgsdgsdgdsg</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>gsdgsdgd</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>879437</t>
+          <t>ssdgsdgdsg</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>ilia</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>valaee</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>0441201423</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>02/18/2023</t>
+          <t>02/20/2023</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added the new book menu and added the add function
</commit_message>
<xml_diff>
--- a/db/user.xlsx
+++ b/db/user.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,12 +468,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>507365</t>
+          <t>381943</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ilia</t>
+          <t>iliya</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -483,7 +483,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0441201425</t>
+          <t>0441201423</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -493,39 +493,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>02/20/2023</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>557690</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>sdfgsgsdf</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>gsdgsdgsdgdsg</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>gsdgsdgd</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>ssdgsdgdsg</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>02/20/2023</t>
+          <t>02/27/2023</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
users & books menu is completed!
</commit_message>
<xml_diff>
--- a/db/user.xlsx
+++ b/db/user.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,38 +465,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>381943</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>iliya</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>valaei</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>0441201423</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>02/27/2023</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added new feature for generating mem cards
</commit_message>
<xml_diff>
--- a/db/user.xlsx
+++ b/db/user.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,6 +465,38 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>444063</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>iliya</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>valaee</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>0441201423</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>09307637377</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>02/28/2023</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
users and books are nearly over but still need some new function and made the issue interface
</commit_message>
<xml_diff>
--- a/db/user.xlsx
+++ b/db/user.xlsx
@@ -1,37 +1,87 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GECKO\git-projects\Library management\db\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{084F289C-EABB-4B77-BA1C-3F3A61CA55AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="3765" yWindow="1935" windowWidth="21600" windowHeight="10980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>Mem ID</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>LAST NAME</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>NUMBER</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>444063</t>
+  </si>
+  <si>
+    <t>iliya</t>
+  </si>
+  <si>
+    <t>valaee</t>
+  </si>
+  <si>
+    <t>0441201423</t>
+  </si>
+  <si>
+    <t>09307637377</t>
+  </si>
+  <si>
+    <t>02/28/2023</t>
+  </si>
+  <si>
+    <t>444|asdfsa|24234|24234|</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +96,44 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,81 +421,59 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="23.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Mem ID</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>NAME</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>LAST NAME</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>NUMBER</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>DATE</t>
-        </is>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>444063</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>iliya</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>valaee</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>0441201423</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>09307637377</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>02/28/2023</t>
-        </is>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
so close to finish need some changes
</commit_message>
<xml_diff>
--- a/db/user.xlsx
+++ b/db/user.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GECKO\git-projects\Library management\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{084F289C-EABB-4B77-BA1C-3F3A61CA55AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE53A08A-8B7E-486D-BA06-C651C13EFEAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3765" yWindow="1935" windowWidth="21600" windowHeight="10980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6330" yWindow="2820" windowWidth="21600" windowHeight="10980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Mem ID</t>
   </si>
@@ -40,6 +40,9 @@
     <t>DATE</t>
   </si>
   <si>
+    <t>history</t>
+  </si>
+  <si>
     <t>444063</t>
   </si>
   <si>
@@ -58,7 +61,31 @@
     <t>02/28/2023</t>
   </si>
   <si>
-    <t>444|asdfsa|24234|24234|</t>
+    <t>Missing|injasdf</t>
+  </si>
+  <si>
+    <t>735554</t>
+  </si>
+  <si>
+    <t>morteza</t>
+  </si>
+  <si>
+    <t>pashaei</t>
+  </si>
+  <si>
+    <t>926010932</t>
+  </si>
+  <si>
+    <t>0926010932</t>
+  </si>
+  <si>
+    <t>03/02/2023</t>
+  </si>
+  <si>
+    <t>Missing</t>
+  </si>
+  <si>
+    <t>balance</t>
   </si>
 </sst>
 </file>
@@ -87,7 +114,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -110,6 +137,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -119,7 +157,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,18 +462,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="7" max="7" width="23.85546875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -452,28 +489,63 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="2" t="s">
         <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
its kinda over(trying to add new things) '
'''
k
</commit_message>
<xml_diff>
--- a/db/user.xlsx
+++ b/db/user.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,7 +478,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>444063</t>
+          <t>915382</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -488,7 +488,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>valaee</t>
+          <t>valaei</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -503,59 +503,17 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>02/28/2023</t>
+          <t>03/03/2023</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Missing|injasdf|injasdf|injasdf|injasdf|injasdf|injasdf|injasdf|injasdf|injasdf|injasdf|injasdf|injasdf|injasdf|injasdf|injasdf|injasdf|injasdf|injasdf</t>
+          <t>||animal</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>140</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>735554</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>morteza</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>pashaei</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>926010932</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>0926010932</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>03/02/2023</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Missing</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>0</t>
+          <t>500</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed inheriting bug and replace os.path with manual path
</commit_message>
<xml_diff>
--- a/db/user.xlsx
+++ b/db/user.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,6 +517,90 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>436637</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>morteza</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>pashaei</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>0441202453</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>09961079096</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>03/03/2023</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>|</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>108171</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ali</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>reza</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>82998798</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0923424145234</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>03/03/2023</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>|</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
was to soon to say its over
</commit_message>
<xml_diff>
--- a/db/user.xlsx
+++ b/db/user.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GECKO\git-projects\Library management\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B13AFF68-2793-4868-925E-08D4185B873C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1C1F85-E3B9-4010-A76F-F8056B019815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2565" yWindow="3630" windowWidth="21600" windowHeight="10980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -415,7 +415,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="L11" sqref="A2:L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>